<commit_message>
With continuous analysis and graphs
</commit_message>
<xml_diff>
--- a/Tumor size.xlsx
+++ b/Tumor size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Dropbox\Stanford\AHPBA\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EDCE3E-2C90-4F15-846B-5138EF659E4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3060BD5-20AA-4A6E-AE90-E2F854595054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7951E5C1-74F4-470E-8A62-F63B6B30B312}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -71,21 +71,9 @@
     <t>Tumor size</t>
   </si>
   <si>
-    <t>82.5 (20-200)</t>
-  </si>
-  <si>
-    <t>45 (10-200)</t>
-  </si>
-  <si>
     <t>Yamao, K., et al 2011 </t>
   </si>
   <si>
-    <t>60.1 (38.0)</t>
-  </si>
-  <si>
-    <t>90.0 (45.8)</t>
-  </si>
-  <si>
     <t>0.001</t>
   </si>
   <si>
@@ -96,12 +84,6 @@
   </si>
   <si>
     <t>Keane 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 (45–131) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B= 52 (30–85) </t>
   </si>
   <si>
     <r>
@@ -119,27 +101,44 @@
     </r>
   </si>
   <si>
-    <t>56 (21)</t>
-  </si>
-  <si>
-    <t>52 (31)</t>
-  </si>
-  <si>
     <t>p- value</t>
+  </si>
+  <si>
+    <t>82.5</t>
+  </si>
+  <si>
+    <t>20-200</t>
+  </si>
+  <si>
+    <t>60.1</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>45–131</t>
+  </si>
+  <si>
+    <t>10-200</t>
+  </si>
+  <si>
+    <t>90.0</t>
+  </si>
+  <si>
+    <t>45.8</t>
+  </si>
+  <si>
+    <t>30–85</t>
+  </si>
+  <si>
+    <t>sd/mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,7 +177,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4931582D-6B83-467A-BD95-DA15043DE9E2}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
@@ -504,7 +503,7 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,13 +526,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -553,15 +558,21 @@
         <v>144</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -579,18 +590,24 @@
         <v>150</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -607,19 +624,25 @@
       <c r="F4" s="1">
         <v>42</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
+      <c r="G4" s="1">
+        <v>56</v>
+      </c>
+      <c r="H4" s="1">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <v>52</v>
+      </c>
+      <c r="J4" s="1">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -639,16 +662,16 @@
       <c r="G5" s="1">
         <v>94</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>54</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -665,14 +688,20 @@
       <c r="F6" s="1">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
+      <c r="G6" s="1">
+        <v>100</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="I6" s="1">
+        <v>52</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>